<commit_message>
Added avg number of moves per game to results
</commit_message>
<xml_diff>
--- a/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
+++ b/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Play 1</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Play1Wins/Play2Wins</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +688,9 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>

</xml_diff>

<commit_message>
Almost done with comps
</commit_message>
<xml_diff>
--- a/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
+++ b/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Play 1</t>
   </si>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,9 +691,15 @@
       <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -706,11 +712,17 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -723,8 +735,8 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="2"/>
       <c r="I9" s="4"/>
@@ -740,11 +752,13 @@
         <v>0.1</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -757,10 +771,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nothing, just removed train files
</commit_message>
<xml_diff>
--- a/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
+++ b/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Play 1</t>
   </si>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,18 +688,10 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -717,12 +709,8 @@
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -756,9 +744,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">

</xml_diff>

<commit_message>
Revert "nothing, just removed train files"
This reverts commit 354652df484a4fbead460bed3918929ce4a44f88.
</commit_message>
<xml_diff>
--- a/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
+++ b/ConnectFourML/ConnectFourML/Results/Comp/CompResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Play 1</t>
   </si>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,10 +688,18 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -709,8 +717,12 @@
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -744,7 +756,9 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">

</xml_diff>